<commit_message>
corrected loop bug in getWFTaskTable, where loop would run over the length of numTrials, rather than the value of numTrials
</commit_message>
<xml_diff>
--- a/proc/Tucker/@binnedDataStructure/trialTableLabels.xlsx
+++ b/proc/Tucker/@binnedDataStructure/trialTableLabels.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>variable name</t>
   </si>
@@ -94,6 +93,30 @@
   </si>
   <si>
     <t>A coding variable indicating which target was used, normally parsed from the value of the go word</t>
+  </si>
+  <si>
+    <t>bumpDir</t>
+  </si>
+  <si>
+    <t>bumpPhase</t>
+  </si>
+  <si>
+    <t>bumpTime</t>
+  </si>
+  <si>
+    <t>tgtOnTime</t>
+  </si>
+  <si>
+    <t>direction of the bump in the room coordinate system</t>
+  </si>
+  <si>
+    <t>what part of the trial was the bump in, e.g hold period bumps = 'H'</t>
+  </si>
+  <si>
+    <t>time after trial start when bump was initiated</t>
+  </si>
+  <si>
+    <t>time after trial start at which reach targets is presented</t>
   </si>
 </sst>
 </file>
@@ -411,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="92.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,6 +540,38 @@
         <v>14</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added getCOTaskTable method to cds. Untested
</commit_message>
<xml_diff>
--- a/proc/Tucker/@binnedDataStructure/trialTableLabels.xlsx
+++ b/proc/Tucker/@binnedDataStructure/trialTableLabels.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>variable name</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>time after trial start at which reach targets is presented</t>
+  </si>
+  <si>
+    <t>bumpID</t>
+  </si>
+  <si>
+    <t>integer indicating target code (1-16)</t>
+  </si>
+  <si>
+    <t>integer indicating bump code (1-16)</t>
   </si>
 </sst>
 </file>
@@ -434,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="92.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,6 +581,22 @@
         <v>30</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>